<commit_message>
test log out completed
</commit_message>
<xml_diff>
--- a/com.espn/src/test/resources/test_data.xlsx
+++ b/com.espn/src/test/resources/test_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadou\IdeaProjects\SeleniumBootcamp\com.espn\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DEC367-592B-41A4-B239-6ECE28112959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B3D4B4-57C3-487C-9CE0-A14B2C938C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{7C60162D-2FF2-49A4-93A8-06B503908C3A}"/>
+    <workbookView xWindow="1608" yWindow="1332" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{7C60162D-2FF2-49A4-93A8-06B503908C3A}"/>
   </bookViews>
   <sheets>
     <sheet name="doSearch" sheetId="1" r:id="rId1"/>

</xml_diff>